<commit_message>
new results. 2021/03/26 17:48
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HANYIIK\Desktop\final_res\MPED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4CA8DC-EC71-4D0D-88D8-6738181AB237}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E710BAE1-126F-3B42-B5C1-570F74D876E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,7 +63,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <family val="2"/>
@@ -67,15 +78,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,6 +109,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -117,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -125,22 +149,27 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,13 +471,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,23 +493,23 @@
         <v>0.40239999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.3548</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.39169999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -488,7 +517,7 @@
         <v>0.41789999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -496,95 +525,95 @@
         <v>0.4738</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.41670000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+        <v>0.4214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>0.3417</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+        <v>0.37019999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0.36309999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B9" s="3">
+        <v>0.37380000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>0.35709999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B10" s="2">
+        <v>0.48330000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.30480000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B11" s="4">
+        <v>0.31669999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>0.32019999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.30480000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B13" s="4">
+        <v>0.30709999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.32379999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B14" s="4">
+        <v>0.33810000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>0.25600000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B15" s="4">
+        <v>0.26190000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>0.34289999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" ht="15">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>0.35239999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" ht="15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -592,7 +621,7 @@
         <v>0.4405</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" ht="15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -600,15 +629,15 @@
         <v>0.42380000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" ht="15">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>0.38329999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" ht="15">
       <c r="A21">
         <v>20</v>
       </c>
@@ -616,23 +645,23 @@
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" ht="15">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>0.3095</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" ht="15">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>0.33810000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" ht="15">
       <c r="A24">
         <v>23</v>
       </c>
@@ -640,7 +669,7 @@
         <v>0.40949999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" ht="15">
       <c r="A25">
         <v>24</v>
       </c>
@@ -648,66 +677,65 @@
         <v>0.40949999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" ht="15">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>0.30830000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" ht="15">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>0.31069999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" ht="15">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>0.23810000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" ht="15">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>0.38450000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" ht="15">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>0.38690000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" ht="15">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>0.33450000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B32">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.36191000000000001</v>
+        <v>0.36872666666666665</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new results. 2021/03/27 12:16
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/MPED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E710BAE1-126F-3B42-B5C1-570F74D876E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2C87C-D2AF-9C47-8ECC-0AA718F85BF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
   </si>
   <si>
     <t>平均</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -71,13 +71,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -90,6 +83,13 @@
       <color rgb="FF9C5700"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -146,10 +146,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -158,12 +158,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="差" xfId="2" builtinId="27"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -489,7 +489,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>0.40239999999999998</v>
       </c>
     </row>
@@ -497,7 +497,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>0.3548</v>
       </c>
     </row>
@@ -505,7 +505,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>0.39169999999999999</v>
       </c>
     </row>
@@ -513,7 +513,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>0.41789999999999999</v>
       </c>
     </row>
@@ -521,7 +521,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>0.4738</v>
       </c>
     </row>
@@ -529,7 +529,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>0.4214</v>
       </c>
     </row>
@@ -537,7 +537,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>0.37019999999999997</v>
       </c>
     </row>
@@ -545,7 +545,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>0.37380000000000002</v>
       </c>
     </row>
@@ -553,7 +553,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>0.48330000000000001</v>
       </c>
     </row>
@@ -602,22 +602,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>0.34289999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>0.35239999999999999</v>
+      <c r="B17" s="5">
+        <v>0.36309999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>0.4405</v>
       </c>
     </row>
@@ -625,15 +625,15 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <v>0.42380000000000001</v>
+      <c r="B19" s="3">
+        <v>0.43330000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>0.38329999999999997</v>
       </c>
     </row>
@@ -641,7 +641,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>0.45600000000000002</v>
       </c>
     </row>
@@ -665,7 +665,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>0.40949999999999998</v>
       </c>
     </row>
@@ -673,7 +673,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>0.40949999999999998</v>
       </c>
     </row>
@@ -705,7 +705,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="3">
         <v>0.38450000000000001</v>
       </c>
     </row>
@@ -713,7 +713,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="3">
         <v>0.38690000000000002</v>
       </c>
     </row>
@@ -726,16 +726,16 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B32">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.36872666666666665</v>
+        <v>0.36943666666666669</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new results. 2021/03/28 15:42
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2C87C-D2AF-9C47-8ECC-0AA718F85BF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BE6DC0-4204-A145-81D1-511871F02BE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,14 +40,14 @@
   </si>
   <si>
     <t>平均</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +81,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -141,7 +149,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -152,23 +160,28 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="警告文本" xfId="4" builtinId="11"/>
     <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -489,7 +502,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.40239999999999998</v>
       </c>
     </row>
@@ -497,7 +510,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.3548</v>
       </c>
     </row>
@@ -505,7 +518,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.39169999999999999</v>
       </c>
     </row>
@@ -513,7 +526,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.41789999999999999</v>
       </c>
     </row>
@@ -521,7 +534,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.4738</v>
       </c>
     </row>
@@ -529,7 +542,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.4214</v>
       </c>
     </row>
@@ -537,7 +550,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>0.37019999999999997</v>
       </c>
     </row>
@@ -545,7 +558,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>0.37380000000000002</v>
       </c>
     </row>
@@ -553,7 +566,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.48330000000000001</v>
       </c>
     </row>
@@ -561,7 +574,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>0.31669999999999998</v>
       </c>
     </row>
@@ -569,7 +582,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.32019999999999998</v>
       </c>
     </row>
@@ -577,7 +590,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>0.30709999999999998</v>
       </c>
     </row>
@@ -585,7 +598,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>0.33810000000000001</v>
       </c>
     </row>
@@ -593,7 +606,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.26190000000000002</v>
       </c>
     </row>
@@ -602,14 +615,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>0.34399999999999997</v>
+        <v>0.35949999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>0.36309999999999998</v>
       </c>
     </row>
@@ -617,7 +630,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.4405</v>
       </c>
     </row>
@@ -625,15 +638,15 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
-        <v>0.43330000000000002</v>
+      <c r="B19" s="2">
+        <v>0.4476</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>0.38329999999999997</v>
       </c>
     </row>
@@ -641,7 +654,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>0.45600000000000002</v>
       </c>
     </row>
@@ -649,31 +662,31 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
-        <v>0.3095</v>
+      <c r="B22" s="3">
+        <v>0.31790000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
-        <v>0.33810000000000001</v>
+      <c r="B23" s="2">
+        <v>0.38329999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
-        <v>0.40949999999999998</v>
+      <c r="B24" s="2">
+        <v>0.42859999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>0.40949999999999998</v>
       </c>
     </row>
@@ -681,15 +694,15 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
-        <v>0.30830000000000002</v>
+      <c r="B26" s="3">
+        <v>0.32140000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>0.31069999999999998</v>
       </c>
     </row>
@@ -697,7 +710,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>0.23810000000000001</v>
       </c>
     </row>
@@ -705,7 +718,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>0.38450000000000001</v>
       </c>
     </row>
@@ -713,7 +726,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>0.38690000000000002</v>
       </c>
     </row>
@@ -721,21 +734,21 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>0.33450000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:2" ht="15">
+      <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="6">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.36943666666666669</v>
+        <v>0.37329000000000001</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new results. 2021/03/29 15:06
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A412D-BF36-8C43-B1F8-C803467D0CAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B0F1AD-D822-6E48-87A0-04C46F971DFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,8 +170,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -510,7 +510,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.3548</v>
       </c>
     </row>
@@ -550,7 +550,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0.37019999999999997</v>
       </c>
     </row>
@@ -558,7 +558,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.37380000000000002</v>
       </c>
     </row>
@@ -574,7 +574,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>0.31669999999999998</v>
       </c>
     </row>
@@ -582,7 +582,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>0.32019999999999998</v>
       </c>
     </row>
@@ -590,7 +590,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>0.30709999999999998</v>
       </c>
     </row>
@@ -598,7 +598,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0.33810000000000001</v>
       </c>
     </row>
@@ -606,7 +606,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>0.26190000000000002</v>
       </c>
     </row>
@@ -614,7 +614,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>0.35949999999999999</v>
       </c>
     </row>
@@ -622,7 +622,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>0.36309999999999998</v>
       </c>
     </row>
@@ -662,7 +662,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>0.31790000000000002</v>
       </c>
     </row>
@@ -694,7 +694,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>0.32140000000000002</v>
       </c>
     </row>
@@ -702,16 +702,16 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
-        <v>0.31069999999999998</v>
+      <c r="B27" s="4">
+        <v>0.32379999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
-        <v>0.23810000000000001</v>
+      <c r="B28" s="4">
+        <v>0.28449999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15">
@@ -734,7 +734,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>0.33450000000000002</v>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37329000000000001</v>
+        <v>0.37527333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/03/30 16:58
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B0F1AD-D822-6E48-87A0-04C46F971DFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733E303-CEB5-324A-87FC-235DC9FE23E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,6 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -484,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -679,7 +678,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.42859999999999998</v>
+        <v>0.43209999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15">
@@ -719,7 +718,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.38450000000000001</v>
+        <v>0.38929999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15">
@@ -744,7 +743,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37527333333333335</v>
+        <v>0.37555000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RELU function. 2021/03/31 19:02
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/MPED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733E303-CEB5-324A-87FC-235DC9FE23E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC85CD25-1ED4-3646-BC9C-0F54A76A9B15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
   </si>
   <si>
     <t>平均</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -59,7 +59,15 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -90,13 +98,6 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -150,16 +151,16 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -168,11 +169,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -484,7 +485,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -726,7 +727,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.38690000000000002</v>
+        <v>0.39169999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15">
@@ -743,11 +744,11 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37555000000000011</v>
+        <v>0.37571000000000004</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new results. 2021/04/01 18:09
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC85CD25-1ED4-3646-BC9C-0F54A76A9B15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F957DE-ED61-7744-B2AF-B9F75EA7AACE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,10 +172,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="差" xfId="2" builtinId="27"/>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -727,7 +727,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.39169999999999999</v>
+        <v>0.39639999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15">
@@ -739,12 +739,12 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="15">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37571000000000004</v>
+        <v>0.37586666666666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results and fixed some bugs. 2021/04/10 15:36
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -1,53 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20338"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/MPED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HANYIIK\Desktop\final_res\MPED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F957DE-ED61-7744-B2AF-B9F75EA7AACE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6D6893-39A1-4D9B-8138-27F1E93256DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>people</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>2 Experts</t>
   </si>
   <si>
+    <t>people</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <t>平均</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +49,39 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -70,36 +91,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -151,31 +147,34 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="差" xfId="2" builtinId="27"/>
@@ -488,267 +487,268 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.40239999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15">
+      <c r="B2" s="3">
+        <v>0.40360000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.3548</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15">
+      <c r="B3" s="4">
+        <v>0.34760000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.39169999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15">
+      <c r="B4" s="4">
+        <v>0.31900000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.41789999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15">
+      <c r="B5" s="3">
+        <v>0.43330000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.4738</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15">
+      <c r="B6" s="3">
+        <v>0.49519999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.4214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15">
+      <c r="B7" s="3">
+        <v>0.41789999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.37019999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15">
+      <c r="B8" s="4">
+        <v>0.31430000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>0.37380000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15">
+        <v>0.39290000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.48330000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15">
+      <c r="B10" s="4">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>0.31669999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15">
+        <v>0.31069999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>0.32019999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15">
+        <v>0.32379999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>0.30709999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15">
+        <v>0.32740000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>0.33810000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15">
+        <v>0.3488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>0.26190000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15">
+        <v>0.3024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
-        <v>0.35949999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15">
+      <c r="B16" s="5">
+        <v>0.35120000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>0.36309999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15">
+      <c r="B17" s="5">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
-        <v>0.4405</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15">
+      <c r="B18" s="3">
+        <v>0.42020000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <v>0.4476</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15">
+      <c r="B19" s="3">
+        <v>0.4214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
-        <v>0.38329999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15">
+      <c r="B20" s="5">
+        <v>0.36430000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
-        <v>0.45600000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15">
+      <c r="B21" s="3">
+        <v>0.47620000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
-        <v>0.31790000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15">
+      <c r="B22" s="5">
+        <v>0.3619</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <v>0.38329999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15">
+      <c r="B23" s="3">
+        <v>0.3952</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <v>0.43209999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15">
+      <c r="B24" s="3">
+        <v>0.44169999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
-        <v>0.40949999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15">
+      <c r="B25" s="3">
+        <v>0.38569999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="4">
-        <v>0.32140000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15">
+        <v>0.33689999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>0.32379999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
-        <v>0.28449999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15">
+      <c r="B28" s="5">
+        <v>0.37980000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
-        <v>0.38929999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15">
+      <c r="B29" s="3">
+        <v>0.38329999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
-        <v>0.39639999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15">
+      <c r="B30" s="5">
+        <v>0.37740000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>0.33450000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15">
-      <c r="A32" s="5" t="s">
+        <v>0.31669999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="6">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37586666666666674</v>
+        <v>0.37225999999999998</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new results. 2021/04/19 18:14
</commit_message>
<xml_diff>
--- a/res/MPED/result.xlsx
+++ b/res/MPED/result.xlsx
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.319</v>
+        <v>0.331</v>
       </c>
     </row>
     <row r="5">
@@ -541,7 +541,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3512</v>
+        <v>0.3762</v>
       </c>
     </row>
     <row r="11">
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3238</v>
+        <v>0.3595</v>
       </c>
     </row>
     <row r="13">

</xml_diff>